<commit_message>
Added first pass of load data
</commit_message>
<xml_diff>
--- a/data/BA_Mapping.xlsx
+++ b/data/BA_Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burl878/Documents/Code/code_repos/ntp_heat_wave_loads/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burl878/Documents/Code/code_repos/nuclear_heat_wave_loads_2024/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2D0F38-EA17-BC49-B0B8-AA73743A9B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE34AD16-A7F7-EE4F-AF44-31DC2A03E5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="1780" windowWidth="24540" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BA_Mapping" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="54">
   <si>
     <t>Interconnection</t>
   </si>
@@ -47,39 +47,12 @@
     <t>AECI</t>
   </si>
   <si>
-    <t>AVA</t>
-  </si>
-  <si>
-    <t>WECC</t>
-  </si>
-  <si>
-    <t>AZPS</t>
-  </si>
-  <si>
-    <t>BANC</t>
-  </si>
-  <si>
-    <t>BPAT</t>
-  </si>
-  <si>
-    <t>CHPD</t>
-  </si>
-  <si>
-    <t>CISO</t>
-  </si>
-  <si>
     <t>CPLE</t>
   </si>
   <si>
-    <t>DOPD</t>
-  </si>
-  <si>
     <t>DUK</t>
   </si>
   <si>
-    <t>EPE</t>
-  </si>
-  <si>
     <t>ERCO</t>
   </si>
   <si>
@@ -95,78 +68,39 @@
     <t>FPL</t>
   </si>
   <si>
-    <t>GCPD</t>
-  </si>
-  <si>
     <t>GVL</t>
   </si>
   <si>
     <t>HST</t>
   </si>
   <si>
-    <t>IID</t>
-  </si>
-  <si>
-    <t>IPCO</t>
-  </si>
-  <si>
     <t>ISNE</t>
   </si>
   <si>
     <t>JEA</t>
   </si>
   <si>
-    <t>LDWP</t>
-  </si>
-  <si>
     <t>LGEE</t>
   </si>
   <si>
     <t>MISO</t>
   </si>
   <si>
-    <t>NEVP</t>
-  </si>
-  <si>
     <t>NSB</t>
   </si>
   <si>
-    <t>NWMT</t>
-  </si>
-  <si>
     <t>NYIS</t>
   </si>
   <si>
-    <t>PACE</t>
-  </si>
-  <si>
-    <t>PACW</t>
-  </si>
-  <si>
-    <t>PGE</t>
-  </si>
-  <si>
     <t>PJM</t>
   </si>
   <si>
-    <t>PNM</t>
-  </si>
-  <si>
-    <t>PSCO</t>
-  </si>
-  <si>
-    <t>PSEI</t>
-  </si>
-  <si>
     <t>SC</t>
   </si>
   <si>
     <t>SCEG</t>
   </si>
   <si>
-    <t>SCL</t>
-  </si>
-  <si>
     <t>SEC</t>
   </si>
   <si>
@@ -176,9 +110,6 @@
     <t>SPA</t>
   </si>
   <si>
-    <t>SRP</t>
-  </si>
-  <si>
     <t>SWPP</t>
   </si>
   <si>
@@ -188,27 +119,9 @@
     <t>TEC</t>
   </si>
   <si>
-    <t>TEPC</t>
-  </si>
-  <si>
-    <t>TIDC</t>
-  </si>
-  <si>
-    <t>TPWR</t>
-  </si>
-  <si>
     <t>TVA</t>
   </si>
   <si>
-    <t>WACM</t>
-  </si>
-  <si>
-    <t>WALC</t>
-  </si>
-  <si>
-    <t>WAUW</t>
-  </si>
-  <si>
     <t>TELL_BA_Code</t>
   </si>
   <si>
@@ -221,18 +134,9 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>IPFE, IPMV, IPTV</t>
-  </si>
-  <si>
-    <t>CIPB, CIPV, CISC, CISD, VEA</t>
-  </si>
-  <si>
     <t>Subregions</t>
   </si>
   <si>
-    <t>NEVP, SPPC</t>
-  </si>
-  <si>
     <t>ISO-NE</t>
   </si>
   <si>
@@ -245,18 +149,9 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>BAs are in Canada and are thus not modeled by TELL</t>
-  </si>
-  <si>
     <t>Name mismatch</t>
   </si>
   <si>
-    <t>BA is not modeled by TELL</t>
-  </si>
-  <si>
-    <t>CPLW</t>
-  </si>
-  <si>
     <t>FTP, KEY, LWU, FMPP, RCU, TCEC</t>
   </si>
   <si>
@@ -272,9 +167,6 @@
     <t>TVA, SMT</t>
   </si>
   <si>
-    <t>YAD</t>
-  </si>
-  <si>
     <t>No match in GridView data</t>
   </si>
   <si>
@@ -284,19 +176,25 @@
     <t>APS, ATSI, AEP, OVEC, DAY, DEO&amp;K, DLCO, CE, PJM, PENELEC, ME, JCPL, PL, PECO, PSEG, BGE, PEPCO, AE, DP&amp;L, UGI, RECO, SMECO, EKPC, DVP</t>
   </si>
   <si>
-    <t>IESO, TE, NB, NS, CORNWALL, NF, BCHA, AESO</t>
-  </si>
-  <si>
     <t>TECO</t>
   </si>
   <si>
-    <t>PAID, PAUT, PAWY</t>
-  </si>
-  <si>
     <t>AEPW, GRDA, OKGE, WFEC, SPS, OMPA, MIDW, SUNC, WERE, KCPL, KACY, EMDE, INDN, SPRM, NPPD, GRIS, OPPD, WAPA, BEPC-SPP</t>
   </si>
   <si>
     <t>EES-EMI, EES-EAI, HE, DEI, SIGE, IPL, NIPS, METC, ITCT, WEC, MIUP, BREC, HMPL, LAGN, CWLD, SMEPA, EES, AMMO, AMIL, CWLP, SIPC, OMUA, CLEC, LAFA, LEPA, MJMEUC, SWPA, XEL, MP, SMMPA, GRE, OTP, ALTW, MEC, HAST, LES, MDU, BEPC-MISO, DPC, ALTE, WPS, MGE, UPPC</t>
+  </si>
+  <si>
+    <t>IESO, TE, NB, NS, CORNWALL, NF</t>
+  </si>
+  <si>
+    <t>BAs are in Canada or Mexico and are thus not modeled by TELL</t>
+  </si>
+  <si>
+    <t>SETH, SERU, SEHA, IPP-REL, MH, SPC, OSC, PS, MPW, GLH, CPLW, YAD, WECC, WBDC-WECC</t>
+  </si>
+  <si>
+    <t>BAs are not modeled by TELL</t>
   </si>
 </sst>
 </file>
@@ -1172,11 +1070,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1186,7 +1084,7 @@
     <col min="3" max="3" width="29.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -1195,19 +1093,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1218,10 +1116,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1235,12 +1133,12 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1248,78 +1146,84 @@
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>61</v>
+      <c r="D4" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>61</v>
+        <v>32</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1333,12 +1237,12 @@
         <v>11</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
@@ -1347,10 +1251,10 @@
         <v>12</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1358,15 +1262,18 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>61</v>
+        <v>32</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -1375,38 +1282,35 @@
         <v>14</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D15" s="5" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1414,16 +1318,13 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>61</v>
+        <v>17</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1431,27 +1332,30 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>61</v>
+      <c r="D18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1459,13 +1363,13 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1473,41 +1377,41 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1515,512 +1419,100 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>61</v>
+      <c r="D24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="204" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="D27" s="5" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>30</v>
+        <v>2</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>31</v>
+      <c r="C29" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>